<commit_message>
Removed unnecessary section of code + report work
</commit_message>
<xml_diff>
--- a/AnDS cw/Report files/Results.xlsx
+++ b/AnDS cw/Report files/Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40111906\Desktop\ands\AnDS cw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Graham\Desktop\uni\yr 3\AnDS\cw\AnDS cw\Report files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
   <si>
     <t>Partition Algorithm</t>
   </si>
@@ -33,12 +33,6 @@
   </si>
   <si>
     <t>Costs</t>
-  </si>
-  <si>
-    <t>fail00002</t>
-  </si>
-  <si>
-    <t>fail00004</t>
   </si>
   <si>
     <t>rand00010</t>
@@ -102,6 +96,9 @@
   </si>
   <si>
     <t>Nodes</t>
+  </si>
+  <si>
+    <t>Sample</t>
   </si>
 </sst>
 </file>
@@ -269,71 +266,65 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$D$4:$D$24</c:f>
+              <c:f>Sheet1!$E$4:$E$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>70</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>90</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>100</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>200</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>300</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>400</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>500</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>600</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>700</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>800</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>900</c:v>
-                </c:pt>
-                <c:pt idx="20">
                   <c:v>1000</c:v>
                 </c:pt>
               </c:numCache>
@@ -341,71 +332,65 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$24</c:f>
+              <c:f>Sheet1!$B$4:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>565.68542494923804</c:v>
+                  <c:v>1488.5795039493601</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>565.68542494923804</c:v>
+                  <c:v>2484.8766403576301</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1488.5795039493601</c:v>
+                  <c:v>3192.6748552584099</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2484.8766403576301</c:v>
+                  <c:v>3424.0696145626298</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3192.6748552584099</c:v>
+                  <c:v>5537.5969839016298</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3424.0696145626298</c:v>
+                  <c:v>5784.5904591610997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5537.5969839016298</c:v>
+                  <c:v>5953.0478016177603</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5784.5904591610997</c:v>
+                  <c:v>7192.3788168320198</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5953.0478016177603</c:v>
+                  <c:v>8413.7986590308792</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7192.3788168320198</c:v>
+                  <c:v>9216.9845398956895</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8413.7986590308792</c:v>
+                  <c:v>15035.6086930045</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9216.9845398956895</c:v>
+                  <c:v>21643.2671138121</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>15035.6086930045</c:v>
+                  <c:v>27494.853462420499</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21643.2671138121</c:v>
+                  <c:v>34313.1652323956</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27494.853462420499</c:v>
+                  <c:v>40707.593545427597</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>34313.1652323956</c:v>
+                  <c:v>45299.042302941503</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>40707.593545427597</c:v>
+                  <c:v>52330.759611480498</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>45299.042302941503</c:v>
+                  <c:v>60033.121931086403</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>52330.759611480498</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>60033.121931086403</c:v>
-                </c:pt>
-                <c:pt idx="20">
                   <c:v>63142.974179637597</c:v>
                 </c:pt>
               </c:numCache>
@@ -441,71 +426,65 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$D$4:$D$24</c:f>
+              <c:f>Sheet1!$E$4:$E$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>70</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>90</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>100</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>200</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>300</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>400</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>500</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>600</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>700</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>800</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>900</c:v>
-                </c:pt>
-                <c:pt idx="20">
                   <c:v>1000</c:v>
                 </c:pt>
               </c:numCache>
@@ -513,72 +492,226 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$C$24</c:f>
+              <c:f>Sheet1!$C$4:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>565.68542494923804</c:v>
+                  <c:v>1471.6987914639899</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>565.68542494923804</c:v>
+                  <c:v>2374.6424304000102</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1471.6987914639899</c:v>
+                  <c:v>3251.0923697307298</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2374.6424304000102</c:v>
+                  <c:v>3393.0560346062798</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3251.0923697307298</c:v>
+                  <c:v>4687.6674121368596</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3393.0560346062798</c:v>
+                  <c:v>5063.7620930165704</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4687.6674121368596</c:v>
+                  <c:v>5049.6422913325696</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5063.7620930165704</c:v>
+                  <c:v>6218.1963091540701</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5049.6422913325696</c:v>
+                  <c:v>6909.9767357512601</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6218.1963091540701</c:v>
+                  <c:v>7529.2607519569401</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6909.9767357512601</c:v>
+                  <c:v>12968.045025850801</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7529.2607519569401</c:v>
+                  <c:v>16958.3961051919</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12968.045025850801</c:v>
+                  <c:v>22644.612934975001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>16958.3961051919</c:v>
+                  <c:v>27996.141660154201</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>22644.612934975001</c:v>
+                  <c:v>33416.341384400897</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>27996.141660154201</c:v>
+                  <c:v>37265.692709761002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>33416.341384400897</c:v>
+                  <c:v>42246.390958001102</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>37265.692709761002</c:v>
+                  <c:v>48802.4124369317</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>42246.390958001102</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>48802.4124369317</c:v>
-                </c:pt>
-                <c:pt idx="20">
                   <c:v>51398.864161755402</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sample</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$E$4:$E$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1577</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2699</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3781</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3727</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5412</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5898</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6883</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8442</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38704</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>76929</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>116481</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>153609</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>188740</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>228962</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>266675</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>311675</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>347699</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>390783</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -594,11 +727,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="278793776"/>
-        <c:axId val="278795736"/>
+        <c:axId val="607391056"/>
+        <c:axId val="607390496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="278793776"/>
+        <c:axId val="607391056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -697,7 +830,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="278795736"/>
+        <c:crossAx val="607390496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -705,7 +838,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="278795736"/>
+        <c:axId val="607390496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -812,7 +945,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="278793776"/>
+        <c:crossAx val="607391056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -997,71 +1130,65 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$D$30:$D$50</c:f>
+              <c:f>Sheet1!$D$30:$D$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>70</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>90</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>100</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>200</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>300</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>400</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>500</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>600</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>700</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>800</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>900</c:v>
-                </c:pt>
-                <c:pt idx="20">
                   <c:v>1000</c:v>
                 </c:pt>
               </c:numCache>
@@ -1069,10 +1196,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$30:$B$50</c:f>
+              <c:f>Sheet1!$B$30:$B$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1107,33 +1234,27 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="20">
                   <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
@@ -1169,71 +1290,65 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$D$30:$D$50</c:f>
+              <c:f>Sheet1!$D$30:$D$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>70</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>90</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>100</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>200</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>300</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>400</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>500</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>600</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>700</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>800</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>900</c:v>
-                </c:pt>
-                <c:pt idx="20">
                   <c:v>1000</c:v>
                 </c:pt>
               </c:numCache>
@@ -1241,10 +1356,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$30:$C$50</c:f>
+              <c:f>Sheet1!$C$30:$C$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1264,48 +1379,42 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>15</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>40</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>89</c:v>
+                  <c:v>261</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>160</c:v>
+                  <c:v>397</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>261</c:v>
+                  <c:v>570</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>397</c:v>
+                  <c:v>802</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>570</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>802</c:v>
-                </c:pt>
-                <c:pt idx="20">
                   <c:v>1025</c:v>
                 </c:pt>
               </c:numCache>
@@ -1322,11 +1431,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="278796520"/>
-        <c:axId val="278796912"/>
+        <c:axId val="607399456"/>
+        <c:axId val="607400016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="278796520"/>
+        <c:axId val="607399456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1429,7 +1538,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="278796912"/>
+        <c:crossAx val="607400016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1437,7 +1546,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="278796912"/>
+        <c:axId val="607400016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1544,7 +1653,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="278796520"/>
+        <c:crossAx val="607399456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2741,16 +2850,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>50987</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>84605</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>116821</xdr:rowOff>
+      <xdr:rowOff>83204</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>65555</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>99173</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>112059</xdr:rowOff>
+      <xdr:rowOff>78442</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3065,10 +3174,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D50"/>
+  <dimension ref="A2:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="C4" sqref="C4:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3078,12 +3187,12 @@
     <col min="3" max="3" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -3091,309 +3200,341 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>565.68542494923804</v>
+        <v>1488.5795039493601</v>
       </c>
       <c r="C4">
-        <v>565.68542494923804</v>
+        <v>1471.6987914639899</v>
       </c>
       <c r="D4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1577</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>565.68542494923804</v>
+        <v>2484.8766403576301</v>
       </c>
       <c r="C5">
-        <v>565.68542494923804</v>
+        <v>2374.6424304000102</v>
       </c>
       <c r="D5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2699</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1488.5795039493601</v>
+        <v>3192.6748552584099</v>
       </c>
       <c r="C6">
-        <v>1471.6987914639899</v>
+        <v>3251.0923697307298</v>
       </c>
       <c r="D6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3781</v>
+      </c>
+      <c r="E6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>2484.8766403576301</v>
+        <v>3424.0696145626298</v>
       </c>
       <c r="C7">
-        <v>2374.6424304000102</v>
+        <v>3393.0560346062798</v>
       </c>
       <c r="D7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3727</v>
+      </c>
+      <c r="E7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>3192.6748552584099</v>
+        <v>5537.5969839016298</v>
       </c>
       <c r="C8">
-        <v>3251.0923697307298</v>
+        <v>4687.6674121368596</v>
       </c>
       <c r="D8">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5412</v>
+      </c>
+      <c r="E8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>3424.0696145626298</v>
+        <v>5784.5904591610997</v>
       </c>
       <c r="C9">
-        <v>3393.0560346062798</v>
+        <v>5063.7620930165704</v>
       </c>
       <c r="D9">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6015</v>
+      </c>
+      <c r="E9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>5537.5969839016298</v>
+        <v>5953.0478016177603</v>
       </c>
       <c r="C10">
-        <v>4687.6674121368596</v>
+        <v>5049.6422913325696</v>
       </c>
       <c r="D10">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5898</v>
+      </c>
+      <c r="E10">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>5784.5904591610997</v>
+        <v>7192.3788168320198</v>
       </c>
       <c r="C11">
-        <v>5063.7620930165704</v>
+        <v>6218.1963091540701</v>
       </c>
       <c r="D11">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6883</v>
+      </c>
+      <c r="E11">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>5953.0478016177603</v>
+        <v>8413.7986590308792</v>
       </c>
       <c r="C12">
-        <v>5049.6422913325696</v>
+        <v>6909.9767357512601</v>
       </c>
       <c r="D12">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8442</v>
+      </c>
+      <c r="E12">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>7192.3788168320198</v>
+        <v>9216.9845398956895</v>
       </c>
       <c r="C13">
-        <v>6218.1963091540701</v>
+        <v>7529.2607519569401</v>
       </c>
       <c r="D13">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38704</v>
+      </c>
+      <c r="E13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>8413.7986590308792</v>
+        <v>15035.6086930045</v>
       </c>
       <c r="C14">
-        <v>6909.9767357512601</v>
+        <v>12968.045025850801</v>
       </c>
       <c r="D14">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>76929</v>
+      </c>
+      <c r="E14">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>9216.9845398956895</v>
+        <v>21643.2671138121</v>
       </c>
       <c r="C15">
-        <v>7529.2607519569401</v>
+        <v>16958.3961051919</v>
       </c>
       <c r="D15">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>116481</v>
+      </c>
+      <c r="E15">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>15035.6086930045</v>
+        <v>27494.853462420499</v>
       </c>
       <c r="C16">
-        <v>12968.045025850801</v>
+        <v>22644.612934975001</v>
       </c>
       <c r="D16">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>153609</v>
+      </c>
+      <c r="E16">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>21643.2671138121</v>
+        <v>34313.1652323956</v>
       </c>
       <c r="C17">
-        <v>16958.3961051919</v>
+        <v>27996.141660154201</v>
       </c>
       <c r="D17">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>188740</v>
+      </c>
+      <c r="E17">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>27494.853462420499</v>
+        <v>40707.593545427597</v>
       </c>
       <c r="C18">
-        <v>22644.612934975001</v>
+        <v>33416.341384400897</v>
       </c>
       <c r="D18">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>228962</v>
+      </c>
+      <c r="E18">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>34313.1652323956</v>
+        <v>45299.042302941503</v>
       </c>
       <c r="C19">
-        <v>27996.141660154201</v>
+        <v>37265.692709761002</v>
       </c>
       <c r="D19">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>266675</v>
+      </c>
+      <c r="E19">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>40707.593545427597</v>
+        <v>52330.759611480498</v>
       </c>
       <c r="C20">
-        <v>33416.341384400897</v>
+        <v>42246.390958001102</v>
       </c>
       <c r="D20">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>311675</v>
+      </c>
+      <c r="E20">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>45299.042302941503</v>
+        <v>60033.121931086403</v>
       </c>
       <c r="C21">
-        <v>37265.692709761002</v>
+        <v>48802.4124369317</v>
       </c>
       <c r="D21">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>347699</v>
+      </c>
+      <c r="E21">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>52330.759611480498</v>
+        <v>63142.974179637597</v>
       </c>
       <c r="C22">
-        <v>42246.390958001102</v>
+        <v>51398.864161755402</v>
       </c>
       <c r="D22">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+        <v>390783</v>
+      </c>
+      <c r="E22">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B23">
-        <v>60033.121931086403</v>
-      </c>
-      <c r="C23">
-        <v>48802.4124369317</v>
-      </c>
-      <c r="D23">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <v>63142.974179637597</v>
-      </c>
-      <c r="C24">
-        <v>51398.864161755402</v>
-      </c>
-      <c r="D24">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>0</v>
       </c>
@@ -3401,10 +3542,10 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -3415,10 +3556,10 @@
         <v>0</v>
       </c>
       <c r="D30">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -3429,10 +3570,10 @@
         <v>0</v>
       </c>
       <c r="D31">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -3443,7 +3584,7 @@
         <v>0</v>
       </c>
       <c r="D32">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3457,7 +3598,7 @@
         <v>0</v>
       </c>
       <c r="D33">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3471,7 +3612,7 @@
         <v>0</v>
       </c>
       <c r="D34">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3485,7 +3626,7 @@
         <v>0</v>
       </c>
       <c r="D35">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3496,10 +3637,10 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36">
-        <v>50</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -3510,10 +3651,10 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -3524,10 +3665,10 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D38">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3538,10 +3679,10 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D39">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3552,10 +3693,10 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D40">
-        <v>90</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3563,13 +3704,13 @@
         <v>14</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C41">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="D41">
-        <v>100</v>
+        <v>300</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3577,13 +3718,13 @@
         <v>15</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C42">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="D42">
-        <v>200</v>
+        <v>400</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3591,13 +3732,13 @@
         <v>16</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C43">
-        <v>40</v>
+        <v>160</v>
       </c>
       <c r="D43">
-        <v>300</v>
+        <v>500</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3605,13 +3746,13 @@
         <v>17</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C44">
-        <v>89</v>
+        <v>261</v>
       </c>
       <c r="D44">
-        <v>400</v>
+        <v>600</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3619,13 +3760,13 @@
         <v>18</v>
       </c>
       <c r="B45">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C45">
-        <v>160</v>
+        <v>397</v>
       </c>
       <c r="D45">
-        <v>500</v>
+        <v>700</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3633,13 +3774,13 @@
         <v>19</v>
       </c>
       <c r="B46">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C46">
-        <v>261</v>
+        <v>570</v>
       </c>
       <c r="D46">
-        <v>600</v>
+        <v>800</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -3647,13 +3788,13 @@
         <v>20</v>
       </c>
       <c r="B47">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C47">
-        <v>397</v>
+        <v>802</v>
       </c>
       <c r="D47">
-        <v>700</v>
+        <v>900</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -3661,40 +3802,12 @@
         <v>21</v>
       </c>
       <c r="B48">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C48">
-        <v>570</v>
+        <v>1025</v>
       </c>
       <c r="D48">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>22</v>
-      </c>
-      <c r="B49">
-        <v>5</v>
-      </c>
-      <c r="C49">
-        <v>802</v>
-      </c>
-      <c r="D49">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>23</v>
-      </c>
-      <c r="B50">
-        <v>5</v>
-      </c>
-      <c r="C50">
-        <v>1025</v>
-      </c>
-      <c r="D50">
         <v>1000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Code comments + report work
</commit_message>
<xml_diff>
--- a/AnDS cw/Report files/Results.xlsx
+++ b/AnDS cw/Report files/Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\napier-mail.napier.ac.uk\students\School of Computing\User Data\40111906\My Profile\Desktop\andscw\AnDS cw\Report files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Graham\Desktop\uni\yr 3\AnDS\cw\AnDS cw\Report files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
-  <si>
-    <t>Partition Algorithm</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
   <si>
     <t>Clark-Wright Algorithm</t>
   </si>
@@ -98,16 +95,16 @@
     <t>Nodes</t>
   </si>
   <si>
-    <t>Sample</t>
-  </si>
-  <si>
     <t>Problem Size</t>
   </si>
   <si>
-    <t>Clarke-Wright Alg.</t>
+    <t>Clarke-Wright Algorithm</t>
   </si>
   <si>
-    <t>Partition Alg.</t>
+    <t>Sample Solution</t>
+  </si>
+  <si>
+    <t>CSP Algorithm</t>
   </si>
 </sst>
 </file>
@@ -115,7 +112,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -158,7 +155,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -212,7 +209,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Costs</a:t>
+              <a:t>Cost</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -262,7 +259,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Partition Alg.</c:v>
+                  <c:v>CSP Algorithm</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -422,7 +419,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Clarke-Wright Alg.</c:v>
+                  <c:v>Clarke-Wright Algorithm</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -582,7 +579,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Sample</c:v>
+                  <c:v>Sample Solution</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -742,11 +739,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="175827880"/>
-        <c:axId val="175871688"/>
+        <c:axId val="604142144"/>
+        <c:axId val="604141584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="175827880"/>
+        <c:axId val="604142144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -849,7 +846,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="175871688"/>
+        <c:crossAx val="604141584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -857,7 +854,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="175871688"/>
+        <c:axId val="604141584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -964,7 +961,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="175827880"/>
+        <c:crossAx val="604142144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1040,7 +1037,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1130,7 +1127,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Partition Algorithm</c:v>
+                  <c:v>CSP Algorithm</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1450,11 +1447,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="175816016"/>
-        <c:axId val="16377960"/>
+        <c:axId val="604149424"/>
+        <c:axId val="604149984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="175816016"/>
+        <c:axId val="604149424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1481,11 +1478,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Node</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> Count</a:t>
+                  <a:t>Problem Size</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1557,7 +1550,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16377960"/>
+        <c:crossAx val="604149984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1565,7 +1558,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="16377960"/>
+        <c:axId val="604149984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1672,7 +1665,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="175816016"/>
+        <c:crossAx val="604149424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1748,7 +1741,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -3195,8 +3188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V30" sqref="V30:V48"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3208,26 +3201,26 @@
   <sheetData>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="4">
         <v>1488.5795039493601</v>
@@ -3260,7 +3253,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="4">
         <v>2484.8766403576301</v>
@@ -3293,7 +3286,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="4">
         <v>3192.6748552584099</v>
@@ -3326,7 +3319,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="4">
         <v>3424.0696145626298</v>
@@ -3359,7 +3352,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="4">
         <v>5537.5969839016298</v>
@@ -3392,7 +3385,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="4">
         <v>5784.5904591610997</v>
@@ -3425,7 +3418,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="4">
         <v>5953.0478016177603</v>
@@ -3458,7 +3451,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="4">
         <v>7192.3788168320198</v>
@@ -3491,7 +3484,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4">
         <v>8413.7986590308792</v>
@@ -3524,7 +3517,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4">
         <v>9216.9845398956895</v>
@@ -3557,7 +3550,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4">
         <v>15035.6086930045</v>
@@ -3590,7 +3583,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4">
         <v>21643.2671138121</v>
@@ -3623,7 +3616,7 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4">
         <v>27494.853462420499</v>
@@ -3656,7 +3649,7 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="4">
         <v>34313.1652323956</v>
@@ -3689,7 +3682,7 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="4">
         <v>40707.593545427597</v>
@@ -3722,7 +3715,7 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="4">
         <v>45299.042302941503</v>
@@ -3755,7 +3748,7 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="4">
         <v>52330.759611480498</v>
@@ -3788,7 +3781,7 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="4">
         <v>60033.121931086403</v>
@@ -3821,7 +3814,7 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="4">
         <v>63142.974179637597</v>
@@ -3854,24 +3847,24 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" t="s">
         <v>0</v>
       </c>
-      <c r="C29" t="s">
-        <v>1</v>
-      </c>
       <c r="D29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O29" s="2"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B30" s="3">
         <v>9.3555390000000002E-2</v>
@@ -3898,7 +3891,7 @@
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B31" s="3">
         <v>6.9764039999999999E-2</v>
@@ -3925,7 +3918,7 @@
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B32" s="3">
         <v>7.6922610000000002E-2</v>
@@ -3952,7 +3945,7 @@
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B33" s="3">
         <v>0.10481603</v>
@@ -3979,7 +3972,7 @@
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B34" s="3">
         <v>8.1605189999999994E-2</v>
@@ -4006,7 +3999,7 @@
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B35" s="3">
         <v>0.10259342</v>
@@ -4033,7 +4026,7 @@
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B36" s="3">
         <v>0.18212031000000001</v>
@@ -4060,7 +4053,7 @@
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B37" s="3">
         <v>0.15784144</v>
@@ -4087,7 +4080,7 @@
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B38" s="3">
         <v>0.19803466</v>
@@ -4114,7 +4107,7 @@
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B39" s="3">
         <v>0.18973430999999999</v>
@@ -4141,7 +4134,7 @@
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B40" s="3">
         <v>0.50362755999999997</v>
@@ -4168,7 +4161,7 @@
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B41" s="3">
         <v>0.90139672000000004</v>
@@ -4195,7 +4188,7 @@
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B42" s="3">
         <v>1.40041547</v>
@@ -4222,7 +4215,7 @@
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B43" s="3">
         <v>1.8205487600000001</v>
@@ -4249,7 +4242,7 @@
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B44" s="3">
         <v>2.2944804300000001</v>
@@ -4276,7 +4269,7 @@
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B45" s="3">
         <v>2.89137793</v>
@@ -4303,7 +4296,7 @@
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B46" s="3">
         <v>3.52011377</v>
@@ -4330,7 +4323,7 @@
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B47" s="3">
         <v>4.1784653299999999</v>
@@ -4357,7 +4350,7 @@
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B48" s="3">
         <v>5.0515837499999998</v>
@@ -4383,7 +4376,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="0" scale="95" orientation="portrait" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>